<commit_message>
Add WhatsApp payment receipt using Fast2SMS template 4587
</commit_message>
<xml_diff>
--- a/Fast2SMS WhatsApp Business Templates API 11-08-2025 12-58-55 pm.xlsx
+++ b/Fast2SMS WhatsApp Business Templates API 11-08-2025 12-58-55 pm.xlsx
@@ -1,21 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11008"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaditya/chords_crm/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73252FF6-77CC-964E-A74C-6257C0A6AD21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="1200" yWindow="3500" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="WhatsApp Templates API" sheetId="1" r:id="rId4"/>
+    <sheet name="WhatsApp Templates API" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1" forceFullCalc="1"/>
+  <calcPr calcId="191029" forceFullCalc="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="38">
   <si>
     <t>message_id</t>
   </si>
@@ -122,21 +139,46 @@
 🎶 Let the music continue without interruption!  
 📞 Contact us at +91 7981585309 | BUTTON: Call (PHONE_NUMBER) - +917981585309</t>
   </si>
+  <si>
+    <t>fee_receipt</t>
+  </si>
+  <si>
+    <t>chords music academy (+917981585309)</t>
+  </si>
+  <si>
+    <t>Var1|Var2|Var3|Var4|Var5|Var6</t>
+  </si>
+  <si>
+    <t>https://www.fast2sms.com/dev/whatsapp?authorization=&lt;YOUR_API_KEY&gt;&amp;message_id=4587&amp;numbers=&lt;MOBILE_NUMBER&gt;&amp;variables_values=Var1|Var2|Var3|Var4|Var5|Var6</t>
+  </si>
+  <si>
+    <t>BODY: Dear {Var1}, 
+Thank you for your payment to Chords Music Academy! 🎵
+💰 Payment Details:
+- Amount: ₹{Var2}
+- Receipt No: {Var3}
+- Package: {Var4}
+- Payment Date: {Var5}
+{Var6}
+🎶 Keep practicing and let your musical journey flourish!
+📞 Contact us at +91 7981585309 | BUTTON: Call (PHONE_NUMBER) - +917981585309</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -159,14 +201,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -456,19 +507,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
-  <dimension ref="A1:J6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -500,7 +548,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2968</v>
       </c>
@@ -532,7 +580,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2969</v>
       </c>
@@ -564,7 +612,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2970</v>
       </c>
@@ -596,7 +644,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2990</v>
       </c>
@@ -622,7 +670,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3004</v>
       </c>
@@ -654,18 +702,40 @@
         <v>32</v>
       </c>
     </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>4587</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7">
+        <v>6</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J7" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
-  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
-  <tableParts count="0"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>